<commit_message>
FIX-latitude longitude dan upload excel
</commit_message>
<xml_diff>
--- a/public/download/template.xlsx
+++ b/public/download/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp8.2\htdocs\teacher-attendance\public\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\laragon\www\hadirin-prakerin\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1253A814-24B6-4F4D-8275-1B704DBE279C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921BD6B3-D826-4651-9B93-79B3A236FBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C656D208-5E2B-4049-A6C1-484C0855109F}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>nama</t>
   </si>
   <si>
-    <t>nip</t>
+    <t>email</t>
   </si>
   <si>
-    <t>email</t>
+    <t>kelas</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +430,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>